<commit_message>
updated model files and documentation
</commit_message>
<xml_diff>
--- a/CKD - SD model/R/data/insideckd splits.xlsx
+++ b/CKD - SD model/R/data/insideckd splits.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csucloudservices-my.sharepoint.com/personal/sally_thompson_mlcsu_nhs_uk/Documents/Documents/1210 Renal NHP/ckd-sd/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="8_{9DB81E37-8154-4D78-99AF-039DD6B6933C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{987658BB-DE32-46D9-83B9-0D6B861DB0DB}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{9DB81E37-8154-4D78-99AF-039DD6B6933C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{56FCFE68-900B-4076-A824-75395B3C9139}"/>
   <bookViews>
-    <workbookView xWindow="-28185" yWindow="495" windowWidth="28155" windowHeight="15000" xr2:uid="{E1767882-6CE0-433F-A3DE-6DC600010D08}"/>
+    <workbookView xWindow="-26745" yWindow="960" windowWidth="23175" windowHeight="11595" xr2:uid="{E1767882-6CE0-433F-A3DE-6DC600010D08}"/>
   </bookViews>
   <sheets>
     <sheet name="for R import" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>proportion</t>
   </si>
@@ -57,6 +57,9 @@
   </si>
   <si>
     <t>diag S3 as pc S3-5</t>
+  </si>
+  <si>
+    <t>undiag S3 as pc undiag</t>
   </si>
 </sst>
 </file>
@@ -138,6 +141,11 @@
         <row r="15">
           <cell r="U15">
             <v>0.90084985835694054</v>
+          </cell>
+        </row>
+        <row r="17">
+          <cell r="U17">
+            <v>0.97988092794087456</v>
           </cell>
         </row>
       </sheetData>
@@ -465,15 +473,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35B039D5-955B-4B4C-AB3D-48916544BF61}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
+    <col min="1" max="1" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -520,6 +528,15 @@
         <v>0.76271186440677963</v>
       </c>
     </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6">
+        <f>[1]Sheet1!$U$17</f>
+        <v>0.97988092794087456</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>